<commit_message>
Update testing XLSX and diagram 1.2
</commit_message>
<xml_diff>
--- a/test/2.2.xlsx
+++ b/test/2.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmob\Dropbox\Documentos\TEC\SEMESTRE 11 - I 2020\Arquitectura de Computadores I (CE4301)\Tareas\Tarea 1\arm-assembly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmob\Desktop\Tarea 1 - Entregable\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15FCACA-0D16-489F-ACBC-480DCF4B5640}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9BBEF2-A911-4B22-A7DE-5DD19A495A2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11145" xr2:uid="{F9B2A648-9E4F-4FDD-B5DE-B57E5DEB4835}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F9B2A648-9E4F-4FDD-B5DE-B57E5DEB4835}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>CHAR BIN</t>
   </si>
   <si>
-    <t>RANDOM BIN</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>DECRYPTION</t>
+  </si>
+  <si>
+    <t>RANDOM BIN (using LFSR with "y")</t>
   </si>
 </sst>
 </file>
@@ -474,54 +474,54 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>67</v>
@@ -554,9 +554,9 @@
         <v>1000011</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>108</v>
@@ -589,9 +589,9 @@
         <v>1101100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>97</v>
@@ -624,9 +624,9 @@
         <v>1100001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>117</v>
@@ -659,9 +659,9 @@
         <v>1110101</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>100</v>
@@ -694,9 +694,9 @@
         <v>1100100</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>101</v>
@@ -729,7 +729,7 @@
         <v>1100101</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2">
         <v>32</v>
@@ -762,9 +762,9 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
         <v>83</v>
@@ -797,9 +797,9 @@
         <v>1010011</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
         <v>104</v>
@@ -832,9 +832,9 @@
         <v>1101000</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2">
         <v>97</v>
@@ -867,9 +867,9 @@
         <v>1100001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>110</v>
@@ -902,9 +902,9 @@
         <v>1101110</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2">
         <v>110</v>
@@ -937,9 +937,9 @@
         <v>1101110</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2">
         <v>111</v>
@@ -972,9 +972,9 @@
         <v>1101111</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2">
         <v>110</v>

</xml_diff>